<commit_message>
Updated with new color settings
</commit_message>
<xml_diff>
--- a/VennOutput/NonTrimmed_Combined_Output.xlsx
+++ b/VennOutput/NonTrimmed_Combined_Output.xlsx
@@ -522,7 +522,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>PFIZER_JANSSEN_NOVAVAX</t>
+          <t>Pfizer_mono_Janssen_Novavax</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -609,7 +609,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>PFIZER_JANSSEN_NOVAVAX</t>
+          <t>Pfizer_mono_Janssen_Novavax</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -696,7 +696,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>PFIZER_JANSSEN_NOVAVAX</t>
+          <t>Pfizer_mono_Janssen_Novavax</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -783,7 +783,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>PFIZER_JANSSEN_NOVAVAX</t>
+          <t>Pfizer_mono_Janssen_Novavax</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -870,7 +870,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>PFIZER_JANSSEN_NOVAVAX</t>
+          <t>Pfizer_mono_Janssen_Novavax</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -957,7 +957,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>PFIZER_JANSSEN_NOVAVAX</t>
+          <t>Pfizer_mono_Janssen_Novavax</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1044,7 +1044,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>PFIZER_JANSSEN_NOVAVAX</t>
+          <t>Pfizer_mono_Janssen_Novavax</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1131,7 +1131,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>JANSSEN_NOVAVAX</t>
+          <t>Janssen_Novavax</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1193,7 +1193,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>JANSSEN_NOVAVAX</t>
+          <t>Janssen_Novavax</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1255,7 +1255,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>JANSSEN_NOVAVAX</t>
+          <t>Janssen_Novavax</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1317,7 +1317,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>JANSSEN_NOVAVAX</t>
+          <t>Janssen_Novavax</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1379,7 +1379,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>PFIZER_PFIZER_BIVALENT_MODERNA_MODERNA_BIVALENT_NOVAVAX</t>
+          <t>Pfizer_mono_Pfizer_bi_Moderna_mono_Moderna_bi_Novavax</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1516,7 +1516,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_MODERNA_MODERNA_BIVALENT_NOVAVAX</t>
+          <t>Pfizer_bi_Moderna_mono_Moderna_bi_Novavax</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1628,7 +1628,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_MODERNA_MODERNA_BIVALENT_NOVAVAX</t>
+          <t>Pfizer_bi_Moderna_mono_Moderna_bi_Novavax</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1740,7 +1740,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>PFIZER_PFIZER_BIVALENT_MODERNA_BIVALENT_NOVAVAX</t>
+          <t>Pfizer_mono_Pfizer_bi_Moderna_bi_Novavax</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1852,7 +1852,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>PFIZER_PFIZER_BIVALENT_MODERNA_BIVALENT_NOVAVAX</t>
+          <t>Pfizer_mono_Pfizer_bi_Moderna_bi_Novavax</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1964,7 +1964,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_MODERNA_BIVALENT_NOVAVAX</t>
+          <t>Pfizer_bi_Moderna_bi_Novavax</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -2051,7 +2051,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_MODERNA_BIVALENT_NOVAVAX</t>
+          <t>Pfizer_bi_Moderna_bi_Novavax</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -2138,7 +2138,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_MODERNA_BIVALENT_NOVAVAX</t>
+          <t>Pfizer_bi_Moderna_bi_Novavax</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -2225,7 +2225,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_MODERNA_BIVALENT_NOVAVAX</t>
+          <t>Pfizer_bi_Moderna_bi_Novavax</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -2312,7 +2312,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_MODERNA_BIVALENT_NOVAVAX</t>
+          <t>Pfizer_bi_Moderna_bi_Novavax</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -2399,7 +2399,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_MODERNA_BIVALENT_NOVAVAX</t>
+          <t>Pfizer_bi_Moderna_bi_Novavax</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -2486,7 +2486,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>MODERNA_BIVALENT_NOVAVAX</t>
+          <t>Moderna_bi_Novavax</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -2548,7 +2548,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_NOVAVAX</t>
+          <t>Pfizer_bi_Novavax</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -2610,7 +2610,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>PFIZER_NOVAVAX</t>
+          <t>Pfizer_mono_Novavax</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -2672,7 +2672,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>PFIZER_NOVAVAX</t>
+          <t>Pfizer_mono_Novavax</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -2734,7 +2734,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>PFIZER_NOVAVAX</t>
+          <t>Pfizer_mono_Novavax</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -2796,7 +2796,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>PFIZER_NOVAVAX</t>
+          <t>Pfizer_mono_Novavax</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -2858,7 +2858,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>PFIZER_NOVAVAX</t>
+          <t>Pfizer_mono_Novavax</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -2920,7 +2920,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>PFIZER_NOVAVAX</t>
+          <t>Pfizer_mono_Novavax</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -2982,7 +2982,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>PFIZER_NOVAVAX</t>
+          <t>Pfizer_mono_Novavax</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -3044,7 +3044,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>PFIZER_NOVAVAX</t>
+          <t>Pfizer_mono_Novavax</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -3106,7 +3106,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>PFIZER_NOVAVAX</t>
+          <t>Pfizer_mono_Novavax</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -3168,7 +3168,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -3205,7 +3205,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -3242,7 +3242,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -3279,7 +3279,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -3316,7 +3316,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -3353,7 +3353,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -3390,7 +3390,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -3427,7 +3427,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -3464,7 +3464,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3501,7 +3501,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3538,7 +3538,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -3575,7 +3575,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3612,7 +3612,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3649,7 +3649,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -3686,7 +3686,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -3723,7 +3723,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -3760,7 +3760,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -3797,7 +3797,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -3834,7 +3834,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -3871,7 +3871,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -3908,7 +3908,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -3945,7 +3945,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -3982,7 +3982,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -4019,7 +4019,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -4056,7 +4056,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -4093,7 +4093,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -4130,7 +4130,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -4167,7 +4167,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -4204,7 +4204,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -4241,7 +4241,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -4278,7 +4278,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -4315,7 +4315,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -4352,7 +4352,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -4389,7 +4389,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -4426,7 +4426,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -4463,7 +4463,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -4500,7 +4500,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -4537,7 +4537,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -4574,7 +4574,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -4611,7 +4611,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -4648,7 +4648,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -4685,7 +4685,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -4722,7 +4722,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -4759,7 +4759,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -4796,7 +4796,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -4833,7 +4833,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -4870,7 +4870,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -4907,7 +4907,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -4944,7 +4944,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -4981,7 +4981,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -5018,7 +5018,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -5055,7 +5055,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -5092,7 +5092,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -5129,7 +5129,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -5166,7 +5166,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -5203,7 +5203,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -5240,7 +5240,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -5277,7 +5277,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -5314,7 +5314,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -5351,7 +5351,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -5388,7 +5388,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -5425,7 +5425,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -5462,7 +5462,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -5499,7 +5499,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -5536,7 +5536,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -5573,7 +5573,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -5610,7 +5610,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -5647,7 +5647,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -5684,7 +5684,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -5721,7 +5721,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -5758,7 +5758,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -5795,7 +5795,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -5832,7 +5832,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -5869,7 +5869,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -5906,7 +5906,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -5943,7 +5943,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -5980,7 +5980,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -6017,7 +6017,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -6054,7 +6054,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -6091,7 +6091,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -6128,7 +6128,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -6165,7 +6165,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -6202,7 +6202,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -6239,7 +6239,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -6276,7 +6276,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -6313,7 +6313,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -6350,7 +6350,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -6387,7 +6387,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -6424,7 +6424,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -6461,7 +6461,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -6498,7 +6498,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -6535,7 +6535,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -6572,7 +6572,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -6609,7 +6609,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -6646,7 +6646,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -6683,7 +6683,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -6720,7 +6720,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -6757,7 +6757,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -6794,7 +6794,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -6831,7 +6831,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -6868,7 +6868,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -6905,7 +6905,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -6942,7 +6942,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -6979,7 +6979,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -7016,7 +7016,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
@@ -7053,7 +7053,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -7090,7 +7090,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -7127,7 +7127,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -7164,7 +7164,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -7201,7 +7201,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -7238,7 +7238,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
@@ -7275,7 +7275,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
@@ -7312,7 +7312,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -7349,7 +7349,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -7386,7 +7386,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
@@ -7423,7 +7423,7 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
@@ -7460,7 +7460,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -7497,7 +7497,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -7534,7 +7534,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -7571,7 +7571,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -7608,7 +7608,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
@@ -7645,7 +7645,7 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
@@ -7682,7 +7682,7 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
@@ -7719,7 +7719,7 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
@@ -7756,7 +7756,7 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
@@ -7793,7 +7793,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -7830,7 +7830,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -7867,7 +7867,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -7904,7 +7904,7 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
@@ -7941,7 +7941,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -7978,7 +7978,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -8015,7 +8015,7 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>NOVAVAX</t>
+          <t>Novavax</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
@@ -8052,7 +8052,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>MODERNA_MODERNA_BIVALENT_JANSSEN</t>
+          <t>Moderna_mono_Moderna_bi_Janssen</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -8139,7 +8139,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>PFIZER_PFIZER_BIVALENT_MODERNA_BIVALENT_JANSSEN</t>
+          <t>Pfizer_mono_Pfizer_bi_Moderna_bi_Janssen</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -8251,7 +8251,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>PFIZER_PFIZER_BIVALENT_MODERNA_BIVALENT_JANSSEN</t>
+          <t>Pfizer_mono_Pfizer_bi_Moderna_bi_Janssen</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
@@ -8363,7 +8363,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>PFIZER_PFIZER_BIVALENT_MODERNA_BIVALENT_JANSSEN</t>
+          <t>Pfizer_mono_Pfizer_bi_Moderna_bi_Janssen</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -8475,7 +8475,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_MODERNA_BIVALENT_JANSSEN</t>
+          <t>Pfizer_bi_Moderna_bi_Janssen</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
@@ -8562,7 +8562,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>PFIZER_MODERNA_BIVALENT_JANSSEN</t>
+          <t>Pfizer_mono_Moderna_bi_Janssen</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
@@ -8649,7 +8649,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>MODERNA_BIVALENT_JANSSEN</t>
+          <t>Moderna_bi_Janssen</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -8711,7 +8711,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>PFIZER_MODERNA_JANSSEN</t>
+          <t>Pfizer_mono_Moderna_mono_Janssen</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -8798,7 +8798,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>PFIZER_PFIZER_BIVALENT_JANSSEN</t>
+          <t>Pfizer_mono_Pfizer_bi_Janssen</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -8885,7 +8885,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>PFIZER_PFIZER_BIVALENT_JANSSEN</t>
+          <t>Pfizer_mono_Pfizer_bi_Janssen</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -8972,7 +8972,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_JANSSEN</t>
+          <t>Pfizer_bi_Janssen</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -9034,7 +9034,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_JANSSEN</t>
+          <t>Pfizer_bi_Janssen</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -9096,7 +9096,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_JANSSEN</t>
+          <t>Pfizer_bi_Janssen</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
@@ -9158,7 +9158,7 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_JANSSEN</t>
+          <t>Pfizer_bi_Janssen</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
@@ -9220,7 +9220,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_JANSSEN</t>
+          <t>Pfizer_bi_Janssen</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
@@ -9282,7 +9282,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>PFIZER_JANSSEN</t>
+          <t>Pfizer_mono_Janssen</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
@@ -9344,7 +9344,7 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>PFIZER_JANSSEN</t>
+          <t>Pfizer_mono_Janssen</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
@@ -9406,7 +9406,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>PFIZER_JANSSEN</t>
+          <t>Pfizer_mono_Janssen</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -9468,7 +9468,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>PFIZER_JANSSEN</t>
+          <t>Pfizer_mono_Janssen</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -9530,7 +9530,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>PFIZER_JANSSEN</t>
+          <t>Pfizer_mono_Janssen</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -9592,7 +9592,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>PFIZER_JANSSEN</t>
+          <t>Pfizer_mono_Janssen</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -9654,7 +9654,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>PFIZER_JANSSEN</t>
+          <t>Pfizer_mono_Janssen</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -9716,7 +9716,7 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>PFIZER_JANSSEN</t>
+          <t>Pfizer_mono_Janssen</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
@@ -9778,7 +9778,7 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>PFIZER_JANSSEN</t>
+          <t>Pfizer_mono_Janssen</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
@@ -9840,7 +9840,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>PFIZER_JANSSEN</t>
+          <t>Pfizer_mono_Janssen</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
@@ -9902,7 +9902,7 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>PFIZER_JANSSEN</t>
+          <t>Pfizer_mono_Janssen</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
@@ -9964,7 +9964,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>PFIZER_JANSSEN</t>
+          <t>Pfizer_mono_Janssen</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
@@ -10026,7 +10026,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>PFIZER_JANSSEN</t>
+          <t>Pfizer_mono_Janssen</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -10088,7 +10088,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>PFIZER_JANSSEN</t>
+          <t>Pfizer_mono_Janssen</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
@@ -10150,7 +10150,7 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>PFIZER_JANSSEN</t>
+          <t>Pfizer_mono_Janssen</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
@@ -10212,7 +10212,7 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>PFIZER_JANSSEN</t>
+          <t>Pfizer_mono_Janssen</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
@@ -10274,7 +10274,7 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>PFIZER_JANSSEN</t>
+          <t>Pfizer_mono_Janssen</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
@@ -10336,7 +10336,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>PFIZER_JANSSEN</t>
+          <t>Pfizer_mono_Janssen</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
@@ -10398,7 +10398,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>PFIZER_JANSSEN</t>
+          <t>Pfizer_mono_Janssen</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
@@ -10460,7 +10460,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
@@ -10497,7 +10497,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
@@ -10534,7 +10534,7 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
@@ -10571,7 +10571,7 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
@@ -10608,7 +10608,7 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
@@ -10645,7 +10645,7 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
@@ -10682,7 +10682,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
@@ -10719,7 +10719,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -10756,7 +10756,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
@@ -10793,7 +10793,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
@@ -10830,7 +10830,7 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
@@ -10867,7 +10867,7 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
@@ -10904,7 +10904,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -10941,7 +10941,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
@@ -10978,7 +10978,7 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
@@ -11015,7 +11015,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
@@ -11052,7 +11052,7 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
@@ -11089,7 +11089,7 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
@@ -11126,7 +11126,7 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
@@ -11163,7 +11163,7 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
@@ -11200,7 +11200,7 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
@@ -11237,7 +11237,7 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
@@ -11274,7 +11274,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -11311,7 +11311,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -11348,7 +11348,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
@@ -11385,7 +11385,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
@@ -11422,7 +11422,7 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
@@ -11459,7 +11459,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
@@ -11496,7 +11496,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -11533,7 +11533,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -11570,7 +11570,7 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
@@ -11607,7 +11607,7 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
@@ -11644,7 +11644,7 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
@@ -11681,7 +11681,7 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
@@ -11718,7 +11718,7 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
@@ -11755,7 +11755,7 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
@@ -11792,7 +11792,7 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
@@ -11829,7 +11829,7 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
@@ -11866,7 +11866,7 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
@@ -11903,7 +11903,7 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
@@ -11940,7 +11940,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -11977,7 +11977,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
@@ -12014,7 +12014,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
@@ -12051,7 +12051,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
@@ -12088,7 +12088,7 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
@@ -12125,7 +12125,7 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>JANSSEN</t>
+          <t>Janssen</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
@@ -12162,7 +12162,7 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>MODERNA_MODERNA_BIVALENT</t>
+          <t>Moderna_mono_Moderna_bi</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
@@ -12224,7 +12224,7 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>PFIZER_PFIZER_BIVALENT_MODERNA_BIVALENT</t>
+          <t>Pfizer_mono_Pfizer_bi_Moderna_bi</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
@@ -12311,7 +12311,7 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>PFIZER_PFIZER_BIVALENT_MODERNA_BIVALENT</t>
+          <t>Pfizer_mono_Pfizer_bi_Moderna_bi</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
@@ -12398,7 +12398,7 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>PFIZER_PFIZER_BIVALENT_MODERNA_BIVALENT</t>
+          <t>Pfizer_mono_Pfizer_bi_Moderna_bi</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
@@ -12485,7 +12485,7 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>PFIZER_PFIZER_BIVALENT_MODERNA_BIVALENT</t>
+          <t>Pfizer_mono_Pfizer_bi_Moderna_bi</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
@@ -12572,7 +12572,7 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>PFIZER_PFIZER_BIVALENT_MODERNA_BIVALENT</t>
+          <t>Pfizer_mono_Pfizer_bi_Moderna_bi</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
@@ -12659,7 +12659,7 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>PFIZER_PFIZER_BIVALENT_MODERNA_BIVALENT</t>
+          <t>Pfizer_mono_Pfizer_bi_Moderna_bi</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
@@ -12746,7 +12746,7 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>PFIZER_PFIZER_BIVALENT_MODERNA_BIVALENT</t>
+          <t>Pfizer_mono_Pfizer_bi_Moderna_bi</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
@@ -12833,7 +12833,7 @@
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>PFIZER_PFIZER_BIVALENT_MODERNA_BIVALENT</t>
+          <t>Pfizer_mono_Pfizer_bi_Moderna_bi</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
@@ -12920,7 +12920,7 @@
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>PFIZER_PFIZER_BIVALENT_MODERNA_BIVALENT</t>
+          <t>Pfizer_mono_Pfizer_bi_Moderna_bi</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
@@ -13007,7 +13007,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_MODERNA_BIVALENT</t>
+          <t>Pfizer_bi_Moderna_bi</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
@@ -13069,7 +13069,7 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_MODERNA_BIVALENT</t>
+          <t>Pfizer_bi_Moderna_bi</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
@@ -13131,7 +13131,7 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_MODERNA_BIVALENT</t>
+          <t>Pfizer_bi_Moderna_bi</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
@@ -13193,7 +13193,7 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_MODERNA_BIVALENT</t>
+          <t>Pfizer_bi_Moderna_bi</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
@@ -13255,7 +13255,7 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_MODERNA_BIVALENT</t>
+          <t>Pfizer_bi_Moderna_bi</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
@@ -13317,7 +13317,7 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_MODERNA_BIVALENT</t>
+          <t>Pfizer_bi_Moderna_bi</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
@@ -13379,7 +13379,7 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_MODERNA_BIVALENT</t>
+          <t>Pfizer_bi_Moderna_bi</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
@@ -13441,7 +13441,7 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_MODERNA_BIVALENT</t>
+          <t>Pfizer_bi_Moderna_bi</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
@@ -13503,7 +13503,7 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_MODERNA_BIVALENT</t>
+          <t>Pfizer_bi_Moderna_bi</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
@@ -13565,7 +13565,7 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_MODERNA_BIVALENT</t>
+          <t>Pfizer_bi_Moderna_bi</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
@@ -13627,7 +13627,7 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_MODERNA_BIVALENT</t>
+          <t>Pfizer_bi_Moderna_bi</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
@@ -13689,7 +13689,7 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_MODERNA_BIVALENT</t>
+          <t>Pfizer_bi_Moderna_bi</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
@@ -13751,7 +13751,7 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_MODERNA_BIVALENT</t>
+          <t>Pfizer_bi_Moderna_bi</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
@@ -13813,7 +13813,7 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_MODERNA_BIVALENT</t>
+          <t>Pfizer_bi_Moderna_bi</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
@@ -13875,7 +13875,7 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_MODERNA_BIVALENT</t>
+          <t>Pfizer_bi_Moderna_bi</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
@@ -13937,7 +13937,7 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_MODERNA_BIVALENT</t>
+          <t>Pfizer_bi_Moderna_bi</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
@@ -13999,7 +13999,7 @@
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_MODERNA_BIVALENT</t>
+          <t>Pfizer_bi_Moderna_bi</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
@@ -14061,7 +14061,7 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_MODERNA_BIVALENT</t>
+          <t>Pfizer_bi_Moderna_bi</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
@@ -14123,7 +14123,7 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_MODERNA_BIVALENT</t>
+          <t>Pfizer_bi_Moderna_bi</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
@@ -14185,7 +14185,7 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_MODERNA_BIVALENT</t>
+          <t>Pfizer_bi_Moderna_bi</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
@@ -14247,7 +14247,7 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_MODERNA_BIVALENT</t>
+          <t>Pfizer_bi_Moderna_bi</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
@@ -14309,7 +14309,7 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_MODERNA_BIVALENT</t>
+          <t>Pfizer_bi_Moderna_bi</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
@@ -14371,7 +14371,7 @@
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_MODERNA_BIVALENT</t>
+          <t>Pfizer_bi_Moderna_bi</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
@@ -14433,7 +14433,7 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_MODERNA_BIVALENT</t>
+          <t>Pfizer_bi_Moderna_bi</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
@@ -14495,7 +14495,7 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_MODERNA_BIVALENT</t>
+          <t>Pfizer_bi_Moderna_bi</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
@@ -14557,7 +14557,7 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_MODERNA_BIVALENT</t>
+          <t>Pfizer_bi_Moderna_bi</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
@@ -14619,7 +14619,7 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_MODERNA_BIVALENT</t>
+          <t>Pfizer_bi_Moderna_bi</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
@@ -14681,7 +14681,7 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT_MODERNA_BIVALENT</t>
+          <t>Pfizer_bi_Moderna_bi</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
@@ -14743,7 +14743,7 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>PFIZER_MODERNA_BIVALENT</t>
+          <t>Pfizer_mono_Moderna_bi</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
@@ -14805,7 +14805,7 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>MODERNA_BIVALENT</t>
+          <t>Moderna_bi</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
@@ -14842,7 +14842,7 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>MODERNA_BIVALENT</t>
+          <t>Moderna_bi</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
@@ -14879,7 +14879,7 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>MODERNA_BIVALENT</t>
+          <t>Moderna_bi</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
@@ -14916,7 +14916,7 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>MODERNA_BIVALENT</t>
+          <t>Moderna_bi</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
@@ -14953,7 +14953,7 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>MODERNA_BIVALENT</t>
+          <t>Moderna_bi</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
@@ -14990,7 +14990,7 @@
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>MODERNA_BIVALENT</t>
+          <t>Moderna_bi</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
@@ -15027,7 +15027,7 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>MODERNA_BIVALENT</t>
+          <t>Moderna_bi</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
@@ -15064,7 +15064,7 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>MODERNA_BIVALENT</t>
+          <t>Moderna_bi</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
@@ -15101,7 +15101,7 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>MODERNA_BIVALENT</t>
+          <t>Moderna_bi</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
@@ -15138,7 +15138,7 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>MODERNA_BIVALENT</t>
+          <t>Moderna_bi</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
@@ -15175,7 +15175,7 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>PFIZER_MODERNA</t>
+          <t>Pfizer_mono_Moderna_mono</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
@@ -15237,7 +15237,7 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>MODERNA</t>
+          <t>Moderna_mono</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
@@ -15274,7 +15274,7 @@
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>MODERNA</t>
+          <t>Moderna_mono</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
@@ -15311,7 +15311,7 @@
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>MODERNA</t>
+          <t>Moderna_mono</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
@@ -15348,7 +15348,7 @@
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>MODERNA</t>
+          <t>Moderna_mono</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
@@ -15385,7 +15385,7 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>MODERNA</t>
+          <t>Moderna_mono</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
@@ -15422,7 +15422,7 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>MODERNA</t>
+          <t>Moderna_mono</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
@@ -15459,7 +15459,7 @@
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>MODERNA</t>
+          <t>Moderna_mono</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
@@ -15496,7 +15496,7 @@
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>MODERNA</t>
+          <t>Moderna_mono</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
@@ -15533,7 +15533,7 @@
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>MODERNA</t>
+          <t>Moderna_mono</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
@@ -15570,7 +15570,7 @@
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>MODERNA</t>
+          <t>Moderna_mono</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
@@ -15607,7 +15607,7 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>MODERNA</t>
+          <t>Moderna_mono</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
@@ -15644,7 +15644,7 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>MODERNA</t>
+          <t>Moderna_mono</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
@@ -15681,7 +15681,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>MODERNA</t>
+          <t>Moderna_mono</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -15718,7 +15718,7 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>PFIZER_PFIZER_BIVALENT</t>
+          <t>Pfizer_mono_Pfizer_bi</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
@@ -15780,7 +15780,7 @@
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>PFIZER_PFIZER_BIVALENT</t>
+          <t>Pfizer_mono_Pfizer_bi</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
@@ -15842,7 +15842,7 @@
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>PFIZER_PFIZER_BIVALENT</t>
+          <t>Pfizer_mono_Pfizer_bi</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
@@ -15904,7 +15904,7 @@
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>PFIZER_PFIZER_BIVALENT</t>
+          <t>Pfizer_mono_Pfizer_bi</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
@@ -15966,7 +15966,7 @@
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>PFIZER_PFIZER_BIVALENT</t>
+          <t>Pfizer_mono_Pfizer_bi</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
@@ -16028,7 +16028,7 @@
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT</t>
+          <t>Pfizer_bi</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
@@ -16065,7 +16065,7 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT</t>
+          <t>Pfizer_bi</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
@@ -16102,7 +16102,7 @@
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT</t>
+          <t>Pfizer_bi</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
@@ -16139,7 +16139,7 @@
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT</t>
+          <t>Pfizer_bi</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
@@ -16176,7 +16176,7 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT</t>
+          <t>Pfizer_bi</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
@@ -16213,7 +16213,7 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT</t>
+          <t>Pfizer_bi</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
@@ -16250,7 +16250,7 @@
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT</t>
+          <t>Pfizer_bi</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
@@ -16287,7 +16287,7 @@
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT</t>
+          <t>Pfizer_bi</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
@@ -16324,7 +16324,7 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT</t>
+          <t>Pfizer_bi</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
@@ -16361,7 +16361,7 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT</t>
+          <t>Pfizer_bi</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
@@ -16398,7 +16398,7 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT</t>
+          <t>Pfizer_bi</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
@@ -16435,7 +16435,7 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT</t>
+          <t>Pfizer_bi</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
@@ -16472,7 +16472,7 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT</t>
+          <t>Pfizer_bi</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
@@ -16509,7 +16509,7 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT</t>
+          <t>Pfizer_bi</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
@@ -16546,7 +16546,7 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT</t>
+          <t>Pfizer_bi</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
@@ -16583,7 +16583,7 @@
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT</t>
+          <t>Pfizer_bi</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
@@ -16620,7 +16620,7 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT</t>
+          <t>Pfizer_bi</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
@@ -16657,7 +16657,7 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT</t>
+          <t>Pfizer_bi</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
@@ -16694,7 +16694,7 @@
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>PFIZER_BIVALENT</t>
+          <t>Pfizer_bi</t>
         </is>
       </c>
       <c r="B333" t="inlineStr">
@@ -16731,7 +16731,7 @@
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>PFIZER</t>
+          <t>Pfizer_mono</t>
         </is>
       </c>
       <c r="B334" t="inlineStr">
@@ -16768,7 +16768,7 @@
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>PFIZER</t>
+          <t>Pfizer_mono</t>
         </is>
       </c>
       <c r="B335" t="inlineStr">
@@ -16805,7 +16805,7 @@
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>PFIZER</t>
+          <t>Pfizer_mono</t>
         </is>
       </c>
       <c r="B336" t="inlineStr">
@@ -16842,7 +16842,7 @@
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>PFIZER</t>
+          <t>Pfizer_mono</t>
         </is>
       </c>
       <c r="B337" t="inlineStr">
@@ -16879,7 +16879,7 @@
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>PFIZER</t>
+          <t>Pfizer_mono</t>
         </is>
       </c>
       <c r="B338" t="inlineStr">
@@ -16916,7 +16916,7 @@
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>PFIZER</t>
+          <t>Pfizer_mono</t>
         </is>
       </c>
       <c r="B339" t="inlineStr">
@@ -16953,7 +16953,7 @@
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>PFIZER</t>
+          <t>Pfizer_mono</t>
         </is>
       </c>
       <c r="B340" t="inlineStr">
@@ -16990,7 +16990,7 @@
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>PFIZER</t>
+          <t>Pfizer_mono</t>
         </is>
       </c>
       <c r="B341" t="inlineStr">
@@ -17027,7 +17027,7 @@
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>PFIZER</t>
+          <t>Pfizer_mono</t>
         </is>
       </c>
       <c r="B342" t="inlineStr">
@@ -17064,7 +17064,7 @@
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>PFIZER</t>
+          <t>Pfizer_mono</t>
         </is>
       </c>
       <c r="B343" t="inlineStr">
@@ -17101,7 +17101,7 @@
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>PFIZER</t>
+          <t>Pfizer_mono</t>
         </is>
       </c>
       <c r="B344" t="inlineStr">
@@ -17138,7 +17138,7 @@
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>PFIZER</t>
+          <t>Pfizer_mono</t>
         </is>
       </c>
       <c r="B345" t="inlineStr">
@@ -17175,7 +17175,7 @@
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>PFIZER</t>
+          <t>Pfizer_mono</t>
         </is>
       </c>
       <c r="B346" t="inlineStr">
@@ -17212,7 +17212,7 @@
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>PFIZER</t>
+          <t>Pfizer_mono</t>
         </is>
       </c>
       <c r="B347" t="inlineStr">
@@ -17249,7 +17249,7 @@
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>PFIZER</t>
+          <t>Pfizer_mono</t>
         </is>
       </c>
       <c r="B348" t="inlineStr">
@@ -17286,7 +17286,7 @@
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>PFIZER</t>
+          <t>Pfizer_mono</t>
         </is>
       </c>
       <c r="B349" t="inlineStr">
@@ -17323,7 +17323,7 @@
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>PFIZER</t>
+          <t>Pfizer_mono</t>
         </is>
       </c>
       <c r="B350" t="inlineStr">
@@ -17360,7 +17360,7 @@
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t>PFIZER</t>
+          <t>Pfizer_mono</t>
         </is>
       </c>
       <c r="B351" t="inlineStr">
@@ -17397,7 +17397,7 @@
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>PFIZER</t>
+          <t>Pfizer_mono</t>
         </is>
       </c>
       <c r="B352" t="inlineStr">
@@ -17434,7 +17434,7 @@
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>PFIZER</t>
+          <t>Pfizer_mono</t>
         </is>
       </c>
       <c r="B353" t="inlineStr">
@@ -17471,7 +17471,7 @@
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>PFIZER</t>
+          <t>Pfizer_mono</t>
         </is>
       </c>
       <c r="B354" t="inlineStr">
@@ -17508,7 +17508,7 @@
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>PFIZER</t>
+          <t>Pfizer_mono</t>
         </is>
       </c>
       <c r="B355" t="inlineStr">

</xml_diff>